<commit_message>
Update graphical output and added eelgrass as habitat variable
</commit_message>
<xml_diff>
--- a/Hab_params.xlsx
+++ b/Hab_params.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="116" documentId="05302AB02B10480D96D8C247B8562C1666E4B080" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{59E14D61-D696-4316-887E-0EAC9044DF2F}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="05302AB02B10480D96D8C247B8562C1666E4B080" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{FA81C55C-5ABD-428D-882D-877A9BC11817}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Parms</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>Effect of Fetch (neg means lower density in high fetch area)</t>
+  </si>
+  <si>
+    <t>beta14</t>
+  </si>
+  <si>
+    <t>Effect of eelgrass</t>
   </si>
 </sst>
 </file>
@@ -241,7 +247,9 @@
           <c:order val="0"/>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -263,41 +271,44 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$13</c:f>
+              <c:f>Sheet1!$G$2:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>-5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>-10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>-15</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>-20</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>-25</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>-30</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>-35</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>-40</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>-45</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>-50</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>-55</c:v>
                 </c:pt>
               </c:numCache>
@@ -305,41 +316,44 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$3:$I$13</c:f>
+              <c:f>Sheet1!$I$2:$I$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1.1912462166123581</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1.2840254166877414</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1.2523227161918642</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1.1051709180756475</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.88249690258459546</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.63762815162177322</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.41686201967850833</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.24659696394160638</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.13199384318783022</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>6.392786120670757E-2</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>2.8015425774221822E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1399,10 +1413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,7 +1508,7 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -1516,7 +1530,7 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -1538,7 +1552,7 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -1560,7 +1574,7 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -1582,7 +1596,7 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>0.05</v>
+        <v>-0.05</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -1604,7 +1618,7 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
@@ -1626,7 +1640,7 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
@@ -1670,7 +1684,7 @@
         <v>26</v>
       </c>
       <c r="B13">
-        <v>-0.15</v>
+        <v>-0.1</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>
@@ -1696,6 +1710,17 @@
       </c>
       <c r="C14" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>0.15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>